<commit_message>
Done with Literally Everything now
</commit_message>
<xml_diff>
--- a/Protokoll 12/Ver 14 Berechnungen.xlsx
+++ b/Protokoll 12/Ver 14 Berechnungen.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="300" yWindow="1800" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
+    <workbookView xWindow="60" yWindow="60" windowWidth="25600" windowHeight="15520" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,6 +16,17 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>AB</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -466,24 +477,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:L10"/>
+  <dimension ref="A2:L10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A10"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
+    <row r="2" spans="1:12">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+    </row>
     <row r="3" spans="1:12">
       <c r="A3">
         <v>0.5</v>
       </c>
       <c r="B3">
-        <v>-89.3</v>
+        <v>89.3</v>
       </c>
       <c r="C3">
-        <f>B3/31.75</f>
-        <v>-2.8125984251968501</v>
+        <f>(B3-A3)/31.75</f>
+        <v>2.7968503937007871</v>
       </c>
       <c r="E3">
         <v>0.1</v>
@@ -494,18 +513,18 @@
       </c>
       <c r="G3">
         <f>C3*F3</f>
-        <v>-5.4349443081562823E-3</v>
+        <v>5.4045134889616781E-3</v>
       </c>
       <c r="I3">
         <f>COS(C3/2)</f>
-        <v>0.16375625445492084</v>
+        <v>0.1715188208377216</v>
       </c>
       <c r="K3">
         <v>0.1</v>
       </c>
       <c r="L3">
         <f>(1/2)*SIN(C3/2)*G3</f>
-        <v>2.6807885376158355E-3</v>
+        <v>2.6622115784684804E-3</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -513,11 +532,11 @@
         <v>0.8</v>
       </c>
       <c r="B4">
-        <v>-84.7</v>
+        <v>84.7</v>
       </c>
       <c r="C4">
-        <f t="shared" ref="C4:C10" si="0">B4/31.75</f>
-        <v>-2.6677165354330707</v>
+        <f t="shared" ref="C4:C10" si="0">(B4-A4)/31.75</f>
+        <v>2.6425196850393702</v>
       </c>
       <c r="E4">
         <v>0.1</v>
@@ -528,18 +547,18 @@
       </c>
       <c r="G4">
         <f t="shared" ref="G4:G10" si="2">C4*F4</f>
-        <v>-5.2506665950418615E-3</v>
+        <v>5.2010735221252914E-3</v>
       </c>
       <c r="I4">
         <f t="shared" ref="I4:I10" si="3">COS(C4/2)</f>
-        <v>0.23472733729308395</v>
+        <v>0.24695482655022133</v>
       </c>
       <c r="K4">
         <v>0.1</v>
       </c>
       <c r="L4">
         <f t="shared" ref="L4:L10" si="4">(1/2)*SIN(C4/2)*G4</f>
-        <v>2.5519847714133952E-3</v>
+        <v>2.5199903184038182E-3</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -547,11 +566,11 @@
         <v>1.2</v>
       </c>
       <c r="B5">
-        <v>-76.599999999999994</v>
+        <v>76.599999999999994</v>
       </c>
       <c r="C5">
         <f t="shared" si="0"/>
-        <v>-2.4125984251968502</v>
+        <v>2.3748031496062989</v>
       </c>
       <c r="E5">
         <v>0.1</v>
@@ -562,18 +581,18 @@
       </c>
       <c r="G5">
         <f t="shared" si="2"/>
-        <v>-4.9351002006401594E-3</v>
+        <v>4.8577879259565021E-3</v>
       </c>
       <c r="I5">
         <f t="shared" si="3"/>
-        <v>0.35647949178329291</v>
+        <v>0.3740709121740784</v>
       </c>
       <c r="K5">
         <v>0.1</v>
       </c>
       <c r="L5">
         <f t="shared" si="4"/>
-        <v>2.3054398260158255E-3</v>
+        <v>2.2525565135646302E-3</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -585,7 +604,7 @@
       </c>
       <c r="C6">
         <f t="shared" si="0"/>
-        <v>2.4850393700787405</v>
+        <v>2.4472440944881892</v>
       </c>
       <c r="E6">
         <v>0.2</v>
@@ -596,18 +615,18 @@
       </c>
       <c r="G6">
         <f t="shared" si="2"/>
-        <v>7.4158717123473123E-3</v>
+        <v>7.3030827889656036E-3</v>
       </c>
       <c r="I6">
         <f t="shared" si="3"/>
-        <v>0.32241217813166384</v>
+        <v>0.34024203733729957</v>
       </c>
       <c r="K6">
         <v>0.1</v>
       </c>
       <c r="L6">
         <f t="shared" si="4"/>
-        <v>3.5099297848370375E-3</v>
+        <v>3.433682746947856E-3</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -619,7 +638,7 @@
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>2.1102362204724407</v>
+        <v>2.0566929133858265</v>
       </c>
       <c r="E7">
         <v>0.3</v>
@@ -630,18 +649,18 @@
       </c>
       <c r="G7">
         <f t="shared" si="2"/>
-        <v>1.0016180957586709E-2</v>
+        <v>9.7620390526927166E-3</v>
       </c>
       <c r="I7">
         <f t="shared" si="3"/>
-        <v>0.49312498264849725</v>
+        <v>0.51623572151961727</v>
       </c>
       <c r="K7">
         <v>0.1</v>
       </c>
       <c r="L7">
         <f t="shared" si="4"/>
-        <v>4.3568307649868524E-3</v>
+        <v>4.1803322962651775E-3</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -653,7 +672,7 @@
       </c>
       <c r="C8">
         <f t="shared" si="0"/>
-        <v>1.6755905511811024</v>
+        <v>1.6062992125984252</v>
       </c>
       <c r="E8">
         <v>0.3</v>
@@ -664,18 +683,18 @@
       </c>
       <c r="G8">
         <f t="shared" si="2"/>
-        <v>9.8103542061545174E-3</v>
+        <v>9.404662866802263E-3</v>
       </c>
       <c r="I8">
         <f t="shared" si="3"/>
-        <v>0.66910293516997188</v>
+        <v>0.69444386815068593</v>
       </c>
       <c r="K8">
         <v>0.1</v>
       </c>
       <c r="L8">
         <f t="shared" si="4"/>
-        <v>3.6453791913421876E-3</v>
+        <v>3.3835479164336145E-3</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -687,7 +706,7 @@
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
-        <v>-1.8803149606299214</v>
+        <v>-1.9370078740157479</v>
       </c>
       <c r="E9">
         <v>0.3</v>
@@ -698,18 +717,18 @@
       </c>
       <c r="G9">
         <f t="shared" si="2"/>
-        <v>-9.9019414908283997E-3</v>
+        <v>-1.0200492490551867E-2</v>
       </c>
       <c r="I9">
         <f t="shared" si="3"/>
-        <v>0.58966084321423684</v>
+        <v>0.56653297906060662</v>
       </c>
       <c r="K9">
         <v>0.1</v>
       </c>
       <c r="L9">
         <f t="shared" si="4"/>
-        <v>3.9986563269306975E-3</v>
+        <v>4.2028021564819631E-3</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -721,7 +740,7 @@
       </c>
       <c r="C10">
         <f t="shared" si="0"/>
-        <v>1.1937007874015748</v>
+        <v>1.1086614173228344</v>
       </c>
       <c r="E10">
         <v>0.3</v>
@@ -732,18 +751,18 @@
       </c>
       <c r="G10">
         <f t="shared" si="2"/>
-        <v>9.6340018227729883E-3</v>
+        <v>8.9476745161374428E-3</v>
       </c>
       <c r="I10">
         <f t="shared" si="3"/>
-        <v>0.82710991979093818</v>
+        <v>0.85025292847342659</v>
       </c>
       <c r="K10">
         <v>0.1</v>
       </c>
       <c r="L10">
         <f t="shared" si="4"/>
-        <v>2.7073481306414625E-3</v>
+        <v>2.354913184180153E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>